<commit_message>
export attendance to spreadsheet completed
Signed-off-by: Sakshi107 <46996938+Sakshi107@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/XLS_FILES/attendance_sheet/attendance_sheet - Wed Apr 21 2021.xlsx
+++ b/XLS_FILES/attendance_sheet/attendance_sheet - Wed Apr 21 2021.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>SrNo</t>
   </si>
@@ -40,7 +40,10 @@
     <t>100.00</t>
   </si>
   <si>
-    <t>133.33</t>
+    <t>66.67</t>
+  </si>
+  <si>
+    <t>50.00</t>
   </si>
   <si>
     <t>1811054</t>
@@ -52,7 +55,7 @@
     <t>25.00</t>
   </si>
   <si>
-    <t>Not a part</t>
+    <t>Not a part of class</t>
   </si>
   <si>
     <t>1811049</t>
@@ -61,7 +64,7 @@
     <t>Shreyas More</t>
   </si>
   <si>
-    <t>33.33</t>
+    <t>16.67</t>
   </si>
   <si>
     <t>1811084</t>
@@ -83,7 +86,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -91,16 +94,40 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <family val="2"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCEA28"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8C00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF73131"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -108,12 +135,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,124 +515,124 @@
     <col min="3" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>8</v>
+      <c r="F2" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="s">
-        <v>13</v>
+      <c r="E3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
+      <c r="E4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
+      <c r="D5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>19</v>
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Download xlsx bug resolved
</commit_message>
<xml_diff>
--- a/XLS_FILES/attendance_sheet/attendance_sheet - Wed Apr 21 2021.xlsx
+++ b/XLS_FILES/attendance_sheet/attendance_sheet - Wed Apr 21 2021.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>SrNo</t>
   </si>
@@ -22,64 +22,67 @@
     <t>Name</t>
   </si>
   <si>
-    <t>test join class</t>
-  </si>
-  <si>
-    <t>copy code</t>
-  </si>
-  <si>
-    <t>css A div</t>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>MIP</t>
+  </si>
+  <si>
+    <t>DSIP</t>
+  </si>
+  <si>
+    <t>CSS</t>
+  </si>
+  <si>
+    <t>1811084</t>
+  </si>
+  <si>
+    <t>Nandita</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>Not a part of class</t>
   </si>
   <si>
     <t>1811053</t>
   </si>
   <si>
-    <t>Sakshi Shelar</t>
+    <t>Sakshi</t>
+  </si>
+  <si>
+    <t>75.00</t>
+  </si>
+  <si>
+    <t>1811001</t>
+  </si>
+  <si>
+    <t>Aditya</t>
+  </si>
+  <si>
+    <t>1811049</t>
+  </si>
+  <si>
+    <t>Shreyas</t>
+  </si>
+  <si>
+    <t>60.00</t>
   </si>
   <si>
     <t>100.00</t>
   </si>
   <si>
-    <t>66.67</t>
-  </si>
-  <si>
-    <t>50.00</t>
-  </si>
-  <si>
-    <t>1811054</t>
-  </si>
-  <si>
-    <t>hiral sheth</t>
-  </si>
-  <si>
-    <t>25.00</t>
-  </si>
-  <si>
-    <t>Not a part of class</t>
-  </si>
-  <si>
-    <t>1811049</t>
-  </si>
-  <si>
-    <t>Shreyas More</t>
-  </si>
-  <si>
-    <t>16.67</t>
-  </si>
-  <si>
-    <t>1811084</t>
-  </si>
-  <si>
-    <t>Nandita</t>
-  </si>
-  <si>
-    <t>0.00</t>
-  </si>
-  <si>
-    <t>1811043</t>
-  </si>
-  <si>
-    <t>Hasti shah</t>
+    <t>1811042</t>
+  </si>
+  <si>
+    <t>Akshit</t>
+  </si>
+  <si>
+    <t>33.33</t>
+  </si>
+  <si>
+    <t>1811012</t>
   </si>
 </sst>
 </file>
@@ -104,7 +107,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,17 +116,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFCEA28"/>
+        <fgColor rgb="FFF73131"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF8C00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF73131"/>
+        <fgColor rgb="FFFCEA28"/>
       </patternFill>
     </fill>
   </fills>
@@ -160,13 +158,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -508,14 +506,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="6" width="15" customWidth="1"/>
+    <col min="3" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -531,31 +529,37 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>10</v>
+      <c r="E2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -565,74 +569,109 @@
       <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>17</v>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>20</v>
+      <c r="G6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>